<commit_message>
There was an issue with the capacity which is hopefully fixed now!
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5263438_ad_unsw_edu_au/Documents/Thesis/Economic modeling/Codes/Economic Vaibility in global market/Abstract Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z5263438/Codes/First paper codes/PV_Manufacturing_Supply_Chain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6919" documentId="8_{BBF11898-3211-DF4A-AA10-89329ADC5A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{993AF8FD-BEB9-E641-94A0-C7E8D8FF3879}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B09749A-4527-9C47-90B1-F420E3BC8F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="19640" xr2:uid="{3B7AC3AD-F491-5542-A882-B648A46824FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" firstSheet="1" activeTab="1" xr2:uid="{3B7AC3AD-F491-5542-A882-B648A46824FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Suppliers" sheetId="1" r:id="rId1"/>
@@ -509,9 +509,6 @@
     <t>PerthM</t>
   </si>
   <si>
-    <t>Capacity_Raw</t>
-  </si>
-  <si>
     <t>Usage in Module</t>
   </si>
   <si>
@@ -609,6 +606,9 @@
   </si>
   <si>
     <t>Preference_Factor</t>
+  </si>
+  <si>
+    <t>Capacity_check</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F15B0C-7CA8-E143-ACF5-A8BEA036ABBA}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -14660,16 +14660,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -14677,7 +14677,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9">
@@ -14687,13 +14687,13 @@
         <v>840</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="9">
         <v>444</v>
@@ -14701,13 +14701,13 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9">
@@ -14717,12 +14717,12 @@
         <v>130</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="9">
         <v>7.56</v>
@@ -14730,13 +14730,13 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="9">
         <v>104.7</v>
@@ -14744,13 +14744,13 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="9">
         <v>79.38</v>
@@ -14758,13 +14758,13 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="9">
         <v>175.8</v>
@@ -14772,13 +14772,13 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B9" s="9">
         <v>50</v>
@@ -14786,12 +14786,12 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" s="9">
         <v>200</v>
@@ -14799,7 +14799,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -14811,8 +14811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD35C22-9DE1-E14C-AC26-DFD036E37569}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14845,16 +14845,16 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>94</v>
@@ -14911,8 +14911,8 @@
         <v>599999999.99999988</v>
       </c>
       <c r="C2">
-        <f>B2+1380</f>
-        <v>600001379.99999988</v>
+        <f>B2</f>
+        <v>599999999.99999988</v>
       </c>
       <c r="D2">
         <f>(0.064*((B2/1000000000)^-0.37))*B2</f>
@@ -14953,8 +14953,8 @@
         <v>599999999.99999988</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C31" si="0">B3+1380</f>
-        <v>600001379.99999988</v>
+        <f t="shared" ref="C3:C31" si="0">B3</f>
+        <v>599999999.99999988</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D31" si="1">(0.064*((B3/1000000000)^-0.37))*B3</f>
@@ -14993,7 +14993,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
@@ -15031,7 +15031,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
@@ -15069,7 +15069,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
@@ -15107,7 +15107,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -15146,7 +15146,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
@@ -15185,7 +15185,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -15224,7 +15224,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
@@ -15263,7 +15263,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
@@ -15302,7 +15302,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
@@ -15341,7 +15341,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
@@ -15380,7 +15380,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
@@ -15419,7 +15419,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
@@ -15458,7 +15458,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
@@ -15497,7 +15497,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
@@ -15536,7 +15536,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
@@ -15575,7 +15575,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -15614,7 +15614,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
@@ -15653,7 +15653,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
@@ -15692,7 +15692,7 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
@@ -15731,7 +15731,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
@@ -15809,7 +15809,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
@@ -15848,7 +15848,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
@@ -15887,7 +15887,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
@@ -15926,7 +15926,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
@@ -15965,7 +15965,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
@@ -16004,7 +16004,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
@@ -16043,7 +16043,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>600001379.99999988</v>
+        <v>599999999.99999988</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
@@ -16303,7 +16303,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -16329,7 +16329,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>79</v>
@@ -16349,7 +16349,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
         <v>84</v>
@@ -16388,15 +16388,15 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="11">
         <v>0.05</v>
@@ -16404,7 +16404,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="11">
         <v>0.05</v>
@@ -16412,7 +16412,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="11">
         <v>0.3</v>
@@ -16420,18 +16420,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="12">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="12">
         <v>0</v>
@@ -16439,7 +16439,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -16476,7 +16476,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -16659,16 +16659,16 @@
         <v>110</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>